<commit_message>
Updated the links in the spreadsheet with GitHub URL for access
</commit_message>
<xml_diff>
--- a/Analysis Artefacts for Dissertation.xlsx
+++ b/Analysis Artefacts for Dissertation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dissertation forks\artefacts\Dissertation-Artefacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C098B3-AC8E-4036-8A87-5E46E39323D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BB1EB5-D75A-4708-A11F-93A00C4C28C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="838" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,9 +344,6 @@
     <t>Name (Click to navigate)</t>
   </si>
   <si>
-    <t>* - The above links for text and message files and are accessed from dropbox location</t>
-  </si>
-  <si>
     <t>* - All the values from researchgate.com website given above are based till the date - 12/08/2022</t>
   </si>
   <si>
@@ -368,31 +365,34 @@
     <t>All Branches</t>
   </si>
   <si>
-    <t>Developer emails send for analysis\Masters research on 'Jenkins' 1.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Masters research on 'Jenkins' 2.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Expert advice on Masters research on 'Jenkins'.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Masters research on 'Wordpress-develop’.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Expert advise on Masters research on 'Wordpress-develop’.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Masters research on 'IdleonCompanion'.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Expert advice on Masters research on 'IdleonCompanion'.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Masters research on 'OpenMW'.msg</t>
-  </si>
-  <si>
-    <t>Developer emails send for analysis\Expert advice on Masters research on 'OpenMW'.msg</t>
+    <t>Jenkins GitHub URL 2</t>
+  </si>
+  <si>
+    <t>Jenkins GitHub URL1</t>
+  </si>
+  <si>
+    <t>Jenkins GitHub URL 3</t>
+  </si>
+  <si>
+    <t>Wordpress GitHub URL 1</t>
+  </si>
+  <si>
+    <t>Wordpress GitHub URL 2</t>
+  </si>
+  <si>
+    <t>IdleonCompanion GitHub URL 1</t>
+  </si>
+  <si>
+    <t>IdleonCompanion GitHub URL 2</t>
+  </si>
+  <si>
+    <t>OpenMW GitHub URL 1</t>
+  </si>
+  <si>
+    <t>OpenMW GitHub URL 2</t>
+  </si>
+  <si>
+    <t>* - The above links for text and message files and are accessed from GitHub (public) location</t>
   </si>
 </sst>
 </file>
@@ -2289,7 +2289,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
@@ -2298,16 +2298,16 @@
         <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2365,7 +2365,7 @@
         <v>43</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I6" s="16">
         <v>749</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -3292,7 +3292,7 @@
       <c r="B6" s="34"/>
       <c r="C6" s="42"/>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>61</v>
@@ -3303,7 +3303,7 @@
       <c r="B7" s="35"/>
       <c r="C7" s="43"/>
       <c r="D7" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>61</v>
@@ -3320,7 +3320,7 @@
         <v>61</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>61</v>
@@ -3331,7 +3331,7 @@
       <c r="B9" s="35"/>
       <c r="C9" s="45"/>
       <c r="D9" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>61</v>
@@ -3348,7 +3348,7 @@
         <v>63</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>61</v>
@@ -3359,7 +3359,7 @@
       <c r="B11" s="35"/>
       <c r="C11" s="39"/>
       <c r="D11" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>61</v>
@@ -3376,7 +3376,7 @@
         <v>63</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>61</v>
@@ -3387,7 +3387,7 @@
       <c r="B13" s="37"/>
       <c r="C13" s="41"/>
       <c r="D13" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>61</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>

</xml_diff>

<commit_message>
Added missing forked repository details
</commit_message>
<xml_diff>
--- a/Analysis Artefacts for Dissertation.xlsx
+++ b/Analysis Artefacts for Dissertation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dissertation forks\artefacts\Dissertation-Artefacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BB1EB5-D75A-4708-A11F-93A00C4C28C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4938C7D-1262-4B45-8AEF-36253CA50580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="838" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="838" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artefact_Index" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="127">
   <si>
     <t>Artefact details in this spreadsheet</t>
   </si>
@@ -393,6 +393,21 @@
   </si>
   <si>
     <t>* - The above links for text and message files and are accessed from GitHub (public) location</t>
+  </si>
+  <si>
+    <t>https://github.com/AnupJacob/openmw.git</t>
+  </si>
+  <si>
+    <t>https://github.com/AnupJacob/wordpress-develop.git</t>
+  </si>
+  <si>
+    <t>https://github.com/AnupJacob/IdleonCompanion.git</t>
+  </si>
+  <si>
+    <t>https://github.com/AnupJacob/jenkins.git</t>
+  </si>
+  <si>
+    <t>Forked Repository from GitHub</t>
   </si>
 </sst>
 </file>
@@ -2238,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,15 +2265,16 @@
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>48</v>
       </c>
@@ -2271,14 +2287,15 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:10" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2292,25 +2309,28 @@
         <v>108</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -2323,26 +2343,29 @@
       <c r="D5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>717</v>
       </c>
-      <c r="G5" s="16">
+      <c r="H5" s="16">
         <v>35</v>
       </c>
-      <c r="H5" s="16">
+      <c r="I5" s="16">
         <v>6</v>
       </c>
-      <c r="I5" s="16">
+      <c r="J5" s="16">
         <v>62</v>
       </c>
-      <c r="J5" s="16">
+      <c r="K5" s="16">
         <v>6918</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -2355,26 +2378,29 @@
       <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>75</v>
       </c>
-      <c r="G6" s="16">
+      <c r="H6" s="16">
         <v>43</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="I6" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="16">
+      <c r="J6" s="16">
         <v>749</v>
       </c>
-      <c r="J6" s="16">
+      <c r="K6" s="16">
         <v>2360</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -2387,26 +2413,29 @@
       <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="9">
         <v>29</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>17</v>
       </c>
-      <c r="G7" s="16">
+      <c r="H7" s="16">
         <v>14</v>
       </c>
-      <c r="H7" s="16">
+      <c r="I7" s="16">
         <v>2</v>
       </c>
-      <c r="I7" s="16">
+      <c r="J7" s="16">
         <v>0</v>
       </c>
-      <c r="J7" s="16">
+      <c r="K7" s="16">
         <v>3217</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -2419,26 +2448,29 @@
       <c r="D8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
         <v>245</v>
       </c>
-      <c r="G8" s="16">
+      <c r="H8" s="16">
         <v>53</v>
       </c>
-      <c r="H8" s="16">
+      <c r="I8" s="16">
         <v>8</v>
       </c>
-      <c r="I8" s="16">
+      <c r="J8" s="16">
         <v>736</v>
       </c>
-      <c r="J8" s="16">
+      <c r="K8" s="16">
         <v>6079</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>105</v>
       </c>
@@ -2451,11 +2483,12 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{8F1B6CEE-41DA-42A6-A654-3EB4F799542A}"/>
@@ -2464,11 +2497,15 @@
     <hyperlink ref="C7" r:id="rId4" xr:uid="{633F35EF-A345-4BFD-B898-CB73D5CC74E4}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{9567F26C-6D69-4997-857B-E668802F32D3}"/>
     <hyperlink ref="C5" r:id="rId6" xr:uid="{F4D5E70E-B87B-4BC2-894A-1096DC6E7E53}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{4CF5F21A-C9FD-4104-A2E6-B97020DFB372}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{3FF4FA0B-8025-4F8A-893D-8236390BDC00}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{7766D620-A9C6-4E65-AAD0-FB76235B6789}"/>
+    <hyperlink ref="E5" r:id="rId10" xr:uid="{160722B6-DCAA-4F40-91DD-1D44E85C42BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -3228,7 +3265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the link issue for GitHub_locations tab in the spreadsheet
</commit_message>
<xml_diff>
--- a/Analysis Artefacts for Dissertation.xlsx
+++ b/Analysis Artefacts for Dissertation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dissertation forks\artefacts\Dissertation-Artefacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B7AB5B-446D-43D7-A3BE-E7CE9C4A5C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408BE97A-09BD-48E0-8CCF-A52ADFF6D640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="838" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artefact_Index" sheetId="1" r:id="rId1"/>
@@ -797,6 +797,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -862,12 +868,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1105,8 +1105,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>693420</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>281940</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1122,8 +1122,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7871460" y="571500"/>
-          <a:ext cx="1927860" cy="1165860"/>
+          <a:off x="9852660" y="701040"/>
+          <a:ext cx="1927860" cy="1310640"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1967,11 +1967,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1986,10 +1986,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45">
+      <c r="A5" s="23">
         <v>1</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1997,10 +1997,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45">
+      <c r="A6" s="23">
         <v>2</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2008,10 +2008,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45">
+      <c r="A7" s="23">
         <v>3</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2019,10 +2019,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45">
+      <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2030,10 +2030,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45">
+      <c r="A9" s="23">
         <v>5</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2041,10 +2041,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45">
+      <c r="A10" s="23">
         <v>6</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2052,10 +2052,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45">
+      <c r="A11" s="23">
         <v>7</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2071,7 +2071,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" location="Project_Information!A1" display="Project_Information" xr:uid="{F1719AA9-09AA-4986-ADA9-EED061315957}"/>
-    <hyperlink ref="B6" location="'GitHub Locations'!A1" display="GitHub_Locations" xr:uid="{FCE686E5-36FC-4F9A-9AFE-7004854CF00A}"/>
+    <hyperlink ref="B6" location="GitHub_Locations!A1" display="GitHub_Locations" xr:uid="{FCE686E5-36FC-4F9A-9AFE-7004854CF00A}"/>
     <hyperlink ref="B7" location="Performance_Analysis!A1" display="Performance_Analysis" xr:uid="{D75256D3-DFB8-4A59-9F0C-2A566D1D8347}"/>
     <hyperlink ref="B8" location="Security_Analysis!A1" display="Security_Analysis" xr:uid="{7D7326ED-590C-48C7-B8A6-DD5992AF9A8A}"/>
     <hyperlink ref="B9" location="Quality_Analysis!A1" display="Quality_Analysis" xr:uid="{8D090394-B645-4FAE-8978-3B1534C71D7C}"/>
@@ -2089,7 +2089,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2105,14 +2105,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -2226,14 +2226,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
@@ -2263,7 +2263,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A8"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,19 +2282,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -2478,19 +2478,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2521,7 +2521,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A9"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,14 +2535,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2666,14 +2666,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2691,7 +2691,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A12"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2705,14 +2705,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
@@ -2903,14 +2903,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2928,7 +2928,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A11"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2942,14 +2942,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -3120,14 +3120,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="16"/>
     </row>
   </sheetData>
@@ -3146,7 +3146,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3161,15 +3161,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3242,15 +3242,15 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3272,8 +3272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,13 +3286,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
@@ -3315,13 +3315,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29">
+      <c r="A5" s="31">
         <v>1</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="39" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -3332,9 +3332,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="12" t="s">
         <v>110</v>
       </c>
@@ -3343,9 +3343,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="8" t="s">
         <v>112</v>
       </c>
@@ -3354,13 +3354,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="29">
+      <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -3371,9 +3371,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="8" t="s">
         <v>114</v>
       </c>
@@ -3382,13 +3382,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
+      <c r="A10" s="31">
         <v>3</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="39" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -3399,9 +3399,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="8" t="s">
         <v>116</v>
       </c>
@@ -3410,13 +3410,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
+      <c r="A12" s="31">
         <v>4</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="41" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -3427,9 +3427,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="13" t="s">
         <v>118</v>
       </c>
@@ -3438,13 +3438,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>